<commit_message>
Implementar Try Catch a sentencias SQL faltantes, nueva tarea  de mejora
Al archivo Listado_de_posibles_Mejoras_funcionales.xlsx se añade un nuevos registro.
</commit_message>
<xml_diff>
--- a/Documentos/Listado_de_posibles_Mejoras_funcionales.xlsx
+++ b/Documentos/Listado_de_posibles_Mejoras_funcionales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://correoiueedu-my.sharepoint.com/personal/ifbedoya_correo_iue_edu_co/Documents/Ing_Sistemas_IUE/2021-2/Dllo Software Orientado a Objetos/Proyecto_SITS/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{604730FF-30A8-4874-93F3-5B593BCB238E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{604730FF-30A8-4874-93F3-5B593BCB238E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADEE145B-C1BC-40E6-802F-4152D8F873AF}"/>
   <bookViews>
-    <workbookView xWindow="16725" yWindow="1530" windowWidth="28800" windowHeight="11385" xr2:uid="{8167C37D-5418-42FF-94FC-D6D04B72E3EF}"/>
+    <workbookView xWindow="14370" yWindow="2550" windowWidth="28800" windowHeight="11385" xr2:uid="{8167C37D-5418-42FF-94FC-D6D04B72E3EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Mejoras" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Implementado</t>
   </si>
@@ -64,6 +64,10 @@
   </si>
   <si>
     <t>Consume campos IDNETITY de la tabla tblProductoxCombo cuando se genera error en el TRY CATCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Limitar la funcionalidad del botón "Ingresar", Ya que si ingresas el nombre de un combo que ya existe te permitirá agregar productos que dicho comobo no tiene.
+- Aún que en la aplicaciòn muestre un valor en la base de datos se recalcula el valor correcto del combo.</t>
   </si>
 </sst>
 </file>
@@ -99,13 +103,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -424,14 +431,15 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="40" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -490,12 +498,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Agregar mejora no prioritaria a la lista, eliminar SQL repetido
</commit_message>
<xml_diff>
--- a/Documentos/Listado_de_posibles_Mejoras_funcionales.xlsx
+++ b/Documentos/Listado_de_posibles_Mejoras_funcionales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://correoiueedu-my.sharepoint.com/personal/ifbedoya_correo_iue_edu_co/Documents/Ing_Sistemas_IUE/2021-2/Dllo Software Orientado a Objetos/Proyecto_SITS/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{604730FF-30A8-4874-93F3-5B593BCB238E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADEE145B-C1BC-40E6-802F-4152D8F873AF}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{604730FF-30A8-4874-93F3-5B593BCB238E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02ED1499-0CE5-4C51-A9C8-7E4EC5466667}"/>
   <bookViews>
-    <workbookView xWindow="14370" yWindow="2550" windowWidth="28800" windowHeight="11385" xr2:uid="{8167C37D-5418-42FF-94FC-D6D04B72E3EF}"/>
+    <workbookView xWindow="3120" yWindow="3720" windowWidth="28800" windowHeight="11325" xr2:uid="{8167C37D-5418-42FF-94FC-D6D04B72E3EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Mejoras" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Implementado</t>
   </si>
@@ -68,6 +68,12 @@
   <si>
     <t xml:space="preserve"> - Limitar la funcionalidad del botón "Ingresar", Ya que si ingresas el nombre de un combo que ya existe te permitirá agregar productos que dicho comobo no tiene.
 - Aún que en la aplicaciòn muestre un valor en la base de datos se recalcula el valor correcto del combo.</t>
+  </si>
+  <si>
+    <t>frmPedido</t>
+  </si>
+  <si>
+    <t>Al buscar un comobo y si no existe aún así deshabilita los botones de buscar y los texBox</t>
   </si>
 </sst>
 </file>
@@ -432,7 +438,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,6 +524,12 @@
       </c>
       <c r="B6" s="2">
         <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Avances para guardar Pedido y producto x pedido
- Cambio en columnas de las tablas para que esten acordé al funcionamiento del ssistema. archivo: 1-Create_tables.sql
- Parametros opcionales en el stprInsertarPedido para que su funcionalidad sirva para crear el pedido y los productos por pedido. archivo: 10-Create_stprInsertarPedido.sql
- Insertar combos de ejemplos para la creación de los pedidos. Archivo: 11-Data_tables_tblCombo_tblProductoxCombo.sql
</commit_message>
<xml_diff>
--- a/Documentos/Listado_de_posibles_Mejoras_funcionales.xlsx
+++ b/Documentos/Listado_de_posibles_Mejoras_funcionales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://correoiueedu-my.sharepoint.com/personal/ifbedoya_correo_iue_edu_co/Documents/Ing_Sistemas_IUE/2021-2/Dllo Software Orientado a Objetos/Proyecto_SITS/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{604730FF-30A8-4874-93F3-5B593BCB238E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02ED1499-0CE5-4C51-A9C8-7E4EC5466667}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{604730FF-30A8-4874-93F3-5B593BCB238E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30265894-09E4-4A53-B3DF-D0CA2F879365}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3720" windowWidth="28800" windowHeight="11325" xr2:uid="{8167C37D-5418-42FF-94FC-D6D04B72E3EF}"/>
+    <workbookView xWindow="1170" yWindow="1770" windowWidth="28800" windowHeight="11385" xr2:uid="{8167C37D-5418-42FF-94FC-D6D04B72E3EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Mejoras" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Exposición FINAL Clase Software Orientado a Objetos
</commit_message>
<xml_diff>
--- a/Documentos/Listado_de_posibles_Mejoras_funcionales.xlsx
+++ b/Documentos/Listado_de_posibles_Mejoras_funcionales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://correoiueedu-my.sharepoint.com/personal/ifbedoya_correo_iue_edu_co/Documents/Ing_Sistemas_IUE/2021-2/Dllo Software Orientado a Objetos/Proyecto_SITS/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{604730FF-30A8-4874-93F3-5B593BCB238E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AA3F69B-21CE-4B9C-8F88-4A366335572D}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{604730FF-30A8-4874-93F3-5B593BCB238E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07B4CACC-58F0-45BD-BE4B-836120CC9681}"/>
   <bookViews>
-    <workbookView xWindow="5265" yWindow="1755" windowWidth="28800" windowHeight="11385" xr2:uid="{8167C37D-5418-42FF-94FC-D6D04B72E3EF}"/>
+    <workbookView xWindow="1170" yWindow="1770" windowWidth="21600" windowHeight="11385" xr2:uid="{8167C37D-5418-42FF-94FC-D6D04B72E3EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Mejoras" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Implementado</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Documentar la instalación de la extensión: rdlc</t>
+  </si>
+  <si>
+    <t>Incluir precio de adornos, canasta, etc</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,6 +583,9 @@
       </c>
       <c r="B10" s="2">
         <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Agregar nuevas opciones de funcionalidades
Pendiente incluir la prioridad y cuales aplicarán para la migración a app móvil
</commit_message>
<xml_diff>
--- a/Documentos/Listado_de_posibles_Mejoras_funcionales.xlsx
+++ b/Documentos/Listado_de_posibles_Mejoras_funcionales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://correoiueedu-my.sharepoint.com/personal/ifbedoya_correo_iue_edu_co/Documents/Ing_Sistemas_IUE/2021-2/Dllo Software Orientado a Objetos/Proyecto_SITS/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{604730FF-30A8-4874-93F3-5B593BCB238E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07B4CACC-58F0-45BD-BE4B-836120CC9681}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="8_{604730FF-30A8-4874-93F3-5B593BCB238E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E48EBFD8-85EB-4FD0-953C-4F9F65F4C911}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1770" windowWidth="21600" windowHeight="11385" xr2:uid="{8167C37D-5418-42FF-94FC-D6D04B72E3EF}"/>
+    <workbookView xWindow="780" yWindow="1380" windowWidth="28800" windowHeight="11385" xr2:uid="{8167C37D-5418-42FF-94FC-D6D04B72E3EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Mejoras" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>Implementado</t>
   </si>
@@ -85,7 +85,63 @@
     <t>Documentar la instalación de la extensión: rdlc</t>
   </si>
   <si>
-    <t>Incluir precio de adornos, canasta, etc</t>
+    <t>Eventos Leave en Código de barras y Nombre del producto que solo se valide sobre el campo que está diligenciado y no sobre los dos</t>
+  </si>
+  <si>
+    <t>frmInventario</t>
+  </si>
+  <si>
+    <t>Nueva Logica de Negocio</t>
+  </si>
+  <si>
+    <t>Incluir precio de adornos, canasta, etc. Se debería cambiar el nombre de producto por nombre de articulo</t>
+  </si>
+  <si>
+    <t>Implementar la logica y funcionamiento del botón de novedad</t>
+  </si>
+  <si>
+    <t>Implementar la funcionalidad de filtrar por el numero del combo</t>
+  </si>
+  <si>
+    <t>Incluir Labels de del total de productos unicos, productos en total en stock y precio total</t>
+  </si>
+  <si>
+    <t>README</t>
+  </si>
+  <si>
+    <t>Congelado</t>
+  </si>
+  <si>
+    <t>BASE DE DATOS</t>
+  </si>
+  <si>
+    <t>Implementar indices adicionales para que las consultas puedan funcionar más rápidamente antes una mayor cantidad de información</t>
+  </si>
+  <si>
+    <t>NUEVO frmCliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - En el frmPedido implementar las opciones para guardar la información del cliente.
+- Implementar una tabla para guardar la información de los clientes.
+- Implementar funcionalidad para editar nombre y dirección del cliente.
+- Utilizar el número de cedular como identificar.
+- Si el cliente existe seleccionarlo en el pedido, sino existe ingresar los datos.</t>
+  </si>
+  <si>
+    <t>- Evitar que el producto adicional sume al total infinitamente el valor cada vez que se ingresa y se sale de la cantidad agregada</t>
+  </si>
+  <si>
+    <t>Habilitar el agregar productos solamente cuando se filtre por un Combo seleccionado</t>
+  </si>
+  <si>
+    <t>Al buscar el combo y seleccionar las filas que esta´n en colos oscuro, la letra se pone blanca y dificulta la visibilidad del dato seleccionado</t>
+  </si>
+  <si>
+    <t>- Evitar cantidades Negativas al añadir un producto adicional
+- Evitar total Negativo</t>
+  </si>
+  <si>
+    <t>Poder modificar un Combo, Añadir o eliminar productos</t>
   </si>
 </sst>
 </file>
@@ -121,17 +177,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,22 +503,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1911248-02AF-437B-A114-97C9677B4F11}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -478,7 +535,7 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>0</v>
       </c>
       <c r="C2" t="s">
@@ -492,7 +549,7 @@
       <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3" t="s">
@@ -506,7 +563,7 @@
       <c r="A4" s="1">
         <v>0</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>0</v>
       </c>
       <c r="C4" t="s">
@@ -516,17 +573,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -534,7 +591,7 @@
       <c r="A6" s="1">
         <v>0</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
       <c r="C6" t="s">
@@ -548,8 +605,11 @@
       <c r="A7" s="1">
         <v>0</v>
       </c>
-      <c r="B7" s="2">
-        <v>0</v>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -559,8 +619,11 @@
       <c r="A8" s="1">
         <v>0</v>
       </c>
-      <c r="B8" s="2">
-        <v>0</v>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
@@ -570,8 +633,11 @@
       <c r="A9" s="1">
         <v>0</v>
       </c>
-      <c r="B9" s="2">
-        <v>0</v>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -581,87 +647,183 @@
       <c r="A10" s="1">
         <v>0</v>
       </c>
-      <c r="B10" s="2">
-        <v>0</v>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0</v>
       </c>
-      <c r="B11" s="2">
-        <v>0</v>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0</v>
       </c>
-      <c r="B12" s="2">
-        <v>0</v>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0</v>
       </c>
-      <c r="B13" s="2">
-        <v>0</v>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0</v>
       </c>
-      <c r="B14" s="2">
-        <v>0</v>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>0</v>
       </c>
-      <c r="B15" s="2">
-        <v>0</v>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>0</v>
       </c>
-      <c r="B16" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>0</v>
       </c>
-      <c r="B17" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0</v>
       </c>
-      <c r="B18" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>0</v>
       </c>
-      <c r="B19" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -670,7 +832,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{3440B080-91F5-41D1-8198-C183264171CA}">
+          <x14:cfRule type="iconSet" priority="3" id="{3440B080-91F5-41D1-8198-C183264171CA}">
             <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -688,6 +850,44 @@
           </x14:cfRule>
           <xm:sqref>A2:A20</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="2" id="{7AB5B377-661F-4944-8EF6-066822351E10}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>-10</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>A21</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{4303AD9A-A720-45DC-A9E8-2E000E8B2605}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>-10</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>A22</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>